<commit_message>
ipdate plantilla and certificates security
</commit_message>
<xml_diff>
--- a/src/assets/plantilla_valorizacion.xlsx
+++ b/src/assets/plantilla_valorizacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sadV2GoogleDrive\backendgoogle\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sistemaaquav2\sadbackendgoogledrive\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A494E2A0-0369-407D-8999-039C0A76BB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF9921E-0A57-4436-A31A-353935FBF9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="923" xr2:uid="{734D1F34-D19D-46E0-BC13-5A1FB95E6648}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="923" activeTab="6" xr2:uid="{734D1F34-D19D-46E0-BC13-5A1FB95E6648}"/>
   </bookViews>
   <sheets>
     <sheet name="configuracion" sheetId="10" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="101">
   <si>
     <t>PARTIDA</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>Cada Columna representa a un título o sub título</t>
-  </si>
-  <si>
-    <t>INDICE DE LA VALORIZACIÓN</t>
   </si>
   <si>
     <t>cs10</t>
@@ -1022,6 +1019,12 @@
       <t>. Fech. Consent. Buena Pro</t>
     </r>
   </si>
+  <si>
+    <t>INDICE / SEPARADOR DE LA VALORIZACIÓN</t>
+  </si>
+  <si>
+    <t>ES SEPARADOR (1) SI; (0) NO</t>
+  </si>
 </sst>
 </file>
 
@@ -1396,7 +1399,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1512,33 +1515,54 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="15" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="10" fontId="15" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1556,42 +1580,21 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="165" fontId="15" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1646,6 +1649,12 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2657,7 +2666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87CACACF-87CF-4126-9F47-FBD0259331BF}">
   <dimension ref="A1:BP35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16:M16"/>
     </sheetView>
   </sheetViews>
@@ -2724,79 +2733,79 @@
     </row>
     <row r="2" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34"/>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
       <c r="J2" s="34"/>
-      <c r="K2" s="55" t="s">
+      <c r="K2" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
       <c r="R2" s="32"/>
       <c r="S2" s="37"/>
-      <c r="T2" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
-      <c r="Z2" s="55"/>
-      <c r="AA2" s="55"/>
+      <c r="T2" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="U2" s="46"/>
+      <c r="V2" s="46"/>
+      <c r="W2" s="46"/>
+      <c r="X2" s="46"/>
+      <c r="Y2" s="46"/>
+      <c r="Z2" s="46"/>
+      <c r="AA2" s="46"/>
       <c r="AB2" s="34"/>
     </row>
     <row r="3" spans="1:28" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34"/>
       <c r="B3" s="28"/>
       <c r="C3" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
       <c r="I3" s="28"/>
       <c r="J3" s="34"/>
       <c r="K3" s="28"/>
       <c r="L3" s="44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M3" s="44"/>
       <c r="N3" s="44"/>
-      <c r="O3" s="45" t="s">
+      <c r="O3" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
       <c r="R3" s="28"/>
       <c r="S3" s="39"/>
       <c r="T3" s="35"/>
       <c r="U3" s="44" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V3" s="44"/>
       <c r="W3" s="44"/>
-      <c r="X3" s="45">
+      <c r="X3" s="43">
         <v>50</v>
       </c>
-      <c r="Y3" s="45"/>
-      <c r="Z3" s="45"/>
+      <c r="Y3" s="43"/>
+      <c r="Z3" s="43"/>
       <c r="AA3" s="35"/>
       <c r="AB3" s="34"/>
     </row>
@@ -2804,41 +2813,41 @@
       <c r="A4" s="34"/>
       <c r="B4" s="28"/>
       <c r="C4" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
       <c r="I4" s="28"/>
       <c r="J4" s="34"/>
       <c r="K4" s="28"/>
       <c r="L4" s="44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M4" s="44"/>
       <c r="N4" s="44"/>
-      <c r="O4" s="46" t="s">
+      <c r="O4" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="50"/>
       <c r="R4" s="28"/>
       <c r="S4" s="39"/>
       <c r="T4" s="35"/>
       <c r="U4" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="V4" s="44"/>
       <c r="W4" s="44"/>
-      <c r="X4" s="46">
+      <c r="X4" s="50">
         <v>500</v>
       </c>
-      <c r="Y4" s="46"/>
-      <c r="Z4" s="46"/>
+      <c r="Y4" s="50"/>
+      <c r="Z4" s="50"/>
       <c r="AA4" s="35"/>
       <c r="AB4" s="34"/>
     </row>
@@ -2846,39 +2855,39 @@
       <c r="A5" s="34"/>
       <c r="B5" s="28"/>
       <c r="C5" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
       <c r="I5" s="28"/>
       <c r="J5" s="34"/>
       <c r="K5" s="28"/>
       <c r="L5" s="44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M5" s="44"/>
       <c r="N5" s="44"/>
-      <c r="O5" s="46" t="s">
+      <c r="O5" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
       <c r="R5" s="28"/>
       <c r="S5" s="39"/>
       <c r="T5" s="35"/>
       <c r="U5" s="44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="V5" s="44"/>
       <c r="W5" s="44"/>
-      <c r="X5" s="47"/>
-      <c r="Y5" s="47"/>
-      <c r="Z5" s="47"/>
+      <c r="X5" s="62"/>
+      <c r="Y5" s="62"/>
+      <c r="Z5" s="62"/>
       <c r="AA5" s="35"/>
       <c r="AB5" s="34"/>
     </row>
@@ -2886,37 +2895,37 @@
       <c r="A6" s="34"/>
       <c r="B6" s="28"/>
       <c r="C6" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
       <c r="I6" s="28"/>
       <c r="J6" s="34"/>
       <c r="K6" s="28"/>
       <c r="L6" s="44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M6" s="44"/>
       <c r="N6" s="44"/>
-      <c r="O6" s="46" t="s">
+      <c r="O6" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
       <c r="R6" s="28"/>
       <c r="S6" s="39"/>
       <c r="T6" s="35"/>
       <c r="U6" s="44"/>
       <c r="V6" s="44"/>
       <c r="W6" s="44"/>
-      <c r="X6" s="48"/>
-      <c r="Y6" s="48"/>
-      <c r="Z6" s="48"/>
+      <c r="X6" s="63"/>
+      <c r="Y6" s="63"/>
+      <c r="Z6" s="63"/>
       <c r="AA6" s="35"/>
       <c r="AB6" s="34"/>
     </row>
@@ -2924,37 +2933,37 @@
       <c r="A7" s="34"/>
       <c r="B7" s="28"/>
       <c r="C7" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
       <c r="I7" s="28"/>
       <c r="J7" s="34"/>
       <c r="K7" s="28"/>
       <c r="L7" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M7" s="44"/>
       <c r="N7" s="44"/>
-      <c r="O7" s="46" t="s">
+      <c r="O7" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="P7" s="46"/>
-      <c r="Q7" s="46"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
       <c r="R7" s="28"/>
       <c r="S7" s="39"/>
       <c r="T7" s="35"/>
       <c r="U7" s="44"/>
       <c r="V7" s="44"/>
       <c r="W7" s="44"/>
-      <c r="X7" s="49"/>
-      <c r="Y7" s="49"/>
-      <c r="Z7" s="49"/>
+      <c r="X7" s="64"/>
+      <c r="Y7" s="64"/>
+      <c r="Z7" s="64"/>
       <c r="AA7" s="35"/>
       <c r="AB7" s="34"/>
     </row>
@@ -2971,15 +2980,15 @@
       <c r="J8" s="34"/>
       <c r="K8" s="28"/>
       <c r="L8" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M8" s="44"/>
       <c r="N8" s="44"/>
-      <c r="O8" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="46"/>
+      <c r="O8" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="50"/>
       <c r="R8" s="28"/>
       <c r="S8" s="39"/>
       <c r="T8" s="35"/>
@@ -3005,15 +3014,15 @@
       <c r="J9" s="34"/>
       <c r="K9" s="28"/>
       <c r="L9" s="44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M9" s="44"/>
       <c r="N9" s="44"/>
-      <c r="O9" s="56">
+      <c r="O9" s="55">
         <v>45272</v>
       </c>
-      <c r="P9" s="56"/>
-      <c r="Q9" s="56"/>
+      <c r="P9" s="55"/>
+      <c r="Q9" s="55"/>
       <c r="R9" s="35" t="str">
         <f>TEXT(O9,"mm/dd/yyyy")</f>
         <v>12/12/2023</v>
@@ -3031,71 +3040,71 @@
     </row>
     <row r="10" spans="1:28" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34"/>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="34"/>
       <c r="K10" s="28"/>
       <c r="L10" s="44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M10" s="44"/>
       <c r="N10" s="44"/>
-      <c r="O10" s="56">
+      <c r="O10" s="55">
         <v>45272</v>
       </c>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="56"/>
+      <c r="P10" s="55"/>
+      <c r="Q10" s="55"/>
       <c r="R10" s="35" t="str">
         <f>TEXT(O10,"mm/dd/yyyy")</f>
         <v>12/12/2023</v>
       </c>
       <c r="S10" s="39"/>
-      <c r="T10" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="U10" s="55"/>
-      <c r="V10" s="55"/>
-      <c r="W10" s="55"/>
-      <c r="X10" s="55"/>
-      <c r="Y10" s="55"/>
-      <c r="Z10" s="55"/>
-      <c r="AA10" s="55"/>
+      <c r="T10" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="U10" s="46"/>
+      <c r="V10" s="46"/>
+      <c r="W10" s="46"/>
+      <c r="X10" s="46"/>
+      <c r="Y10" s="46"/>
+      <c r="Z10" s="46"/>
+      <c r="AA10" s="46"/>
       <c r="AB10" s="34"/>
     </row>
     <row r="11" spans="1:28" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34"/>
       <c r="B11" s="28"/>
       <c r="C11" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="44"/>
-      <c r="E11" s="45" t="s">
+      <c r="E11" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
       <c r="I11" s="28"/>
       <c r="J11" s="34"/>
       <c r="K11" s="28"/>
       <c r="L11" s="44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M11" s="44"/>
       <c r="N11" s="44"/>
-      <c r="O11" s="56">
+      <c r="O11" s="55">
         <v>45273</v>
       </c>
-      <c r="P11" s="56"/>
-      <c r="Q11" s="56"/>
+      <c r="P11" s="55"/>
+      <c r="Q11" s="55"/>
       <c r="R11" s="35" t="str">
         <f>TEXT(O11,"mm/dd/yyyy")</f>
         <v>12/13/2023</v>
@@ -3103,15 +3112,15 @@
       <c r="S11" s="39"/>
       <c r="T11" s="28"/>
       <c r="U11" s="44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="V11" s="44"/>
       <c r="W11" s="44"/>
-      <c r="X11" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y11" s="43"/>
-      <c r="Z11" s="43"/>
+      <c r="X11" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y11" s="47"/>
+      <c r="Z11" s="47"/>
       <c r="AA11" s="28"/>
       <c r="AB11" s="34"/>
     </row>
@@ -3119,28 +3128,28 @@
       <c r="A12" s="34"/>
       <c r="B12" s="28"/>
       <c r="C12" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="44"/>
-      <c r="E12" s="46" t="s">
+      <c r="E12" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
       <c r="I12" s="28"/>
       <c r="J12" s="34"/>
       <c r="K12" s="28"/>
       <c r="L12" s="44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M12" s="44"/>
       <c r="N12" s="44"/>
-      <c r="O12" s="57">
+      <c r="O12" s="56">
         <v>90</v>
       </c>
-      <c r="P12" s="57"/>
-      <c r="Q12" s="57"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="56"/>
       <c r="R12" s="28"/>
       <c r="S12" s="37"/>
       <c r="T12" s="28"/>
@@ -3150,9 +3159,9 @@
       </c>
       <c r="V12" s="44"/>
       <c r="W12" s="44"/>
-      <c r="X12" s="63"/>
-      <c r="Y12" s="63"/>
-      <c r="Z12" s="63"/>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="48"/>
+      <c r="Z12" s="48"/>
       <c r="AA12" s="28"/>
       <c r="AB12" s="34"/>
     </row>
@@ -3169,15 +3178,15 @@
       <c r="J13" s="34"/>
       <c r="K13" s="28"/>
       <c r="L13" s="44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M13" s="44"/>
       <c r="N13" s="28"/>
-      <c r="O13" s="57">
+      <c r="O13" s="56">
         <v>90</v>
       </c>
-      <c r="P13" s="57"/>
-      <c r="Q13" s="57"/>
+      <c r="P13" s="56"/>
+      <c r="Q13" s="56"/>
       <c r="R13" s="28"/>
       <c r="S13" s="37"/>
       <c r="T13" s="28"/>
@@ -3187,9 +3196,9 @@
       </c>
       <c r="V13" s="44"/>
       <c r="W13" s="44"/>
-      <c r="X13" s="63"/>
-      <c r="Y13" s="63"/>
-      <c r="Z13" s="63"/>
+      <c r="X13" s="48"/>
+      <c r="Y13" s="48"/>
+      <c r="Z13" s="48"/>
       <c r="AA13" s="28"/>
       <c r="AB13" s="34"/>
     </row>
@@ -3206,53 +3215,53 @@
       <c r="J14" s="34"/>
       <c r="K14" s="28"/>
       <c r="L14" s="44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M14" s="44"/>
       <c r="N14" s="28"/>
-      <c r="O14" s="57">
+      <c r="O14" s="56">
         <v>90</v>
       </c>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="57"/>
+      <c r="P14" s="56"/>
+      <c r="Q14" s="56"/>
       <c r="R14" s="28"/>
       <c r="S14" s="37"/>
       <c r="T14" s="28"/>
       <c r="U14" s="44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V14" s="44"/>
       <c r="W14" s="44"/>
-      <c r="X14" s="63"/>
-      <c r="Y14" s="63"/>
-      <c r="Z14" s="63"/>
+      <c r="X14" s="48"/>
+      <c r="Y14" s="48"/>
+      <c r="Z14" s="48"/>
       <c r="AA14" s="28"/>
       <c r="AB14" s="34"/>
     </row>
     <row r="15" spans="1:28" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="34"/>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
       <c r="J15" s="34"/>
       <c r="K15" s="28"/>
       <c r="L15" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M15" s="31"/>
       <c r="N15" s="31"/>
-      <c r="O15" s="57">
+      <c r="O15" s="56">
         <v>90</v>
       </c>
-      <c r="P15" s="57"/>
-      <c r="Q15" s="57"/>
+      <c r="P15" s="56"/>
+      <c r="Q15" s="56"/>
       <c r="R15" s="28"/>
       <c r="S15" s="37"/>
       <c r="T15" s="37"/>
@@ -3269,40 +3278,40 @@
       <c r="A16" s="34"/>
       <c r="B16" s="28"/>
       <c r="C16" s="44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D16" s="44"/>
       <c r="E16" s="44"/>
-      <c r="F16" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
+      <c r="F16" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
       <c r="I16" s="28"/>
       <c r="J16" s="34"/>
       <c r="K16" s="28"/>
       <c r="L16" s="44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M16" s="44"/>
       <c r="N16" s="28"/>
-      <c r="O16" s="57">
+      <c r="O16" s="56">
         <v>90</v>
       </c>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="57"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="56"/>
       <c r="R16" s="28"/>
       <c r="S16" s="37"/>
-      <c r="T16" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="U16" s="55"/>
-      <c r="V16" s="55"/>
-      <c r="W16" s="55"/>
-      <c r="X16" s="55"/>
-      <c r="Y16" s="55"/>
-      <c r="Z16" s="55"/>
-      <c r="AA16" s="55"/>
+      <c r="T16" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="U16" s="46"/>
+      <c r="V16" s="46"/>
+      <c r="W16" s="46"/>
+      <c r="X16" s="46"/>
+      <c r="Y16" s="46"/>
+      <c r="Z16" s="46"/>
+      <c r="AA16" s="46"/>
       <c r="AB16" s="34"/>
     </row>
     <row r="17" spans="1:28" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3314,91 +3323,91 @@
       </c>
       <c r="D17" s="44"/>
       <c r="E17" s="44"/>
-      <c r="F17" s="46" t="s">
+      <c r="F17" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
       <c r="I17" s="28"/>
       <c r="J17" s="34"/>
       <c r="K17" s="28"/>
       <c r="L17" s="44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M17" s="44"/>
       <c r="N17" s="44"/>
-      <c r="O17" s="46" t="s">
+      <c r="O17" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="46"/>
+      <c r="P17" s="50"/>
+      <c r="Q17" s="50"/>
       <c r="R17" s="28"/>
       <c r="S17" s="37"/>
       <c r="T17" s="28"/>
       <c r="U17" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="V17" s="44"/>
       <c r="W17" s="44"/>
-      <c r="X17" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y17" s="43"/>
-      <c r="Z17" s="43"/>
+      <c r="X17" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y17" s="47"/>
+      <c r="Z17" s="47"/>
       <c r="AA17" s="28"/>
       <c r="AB17" s="34"/>
     </row>
     <row r="18" spans="1:28" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="34"/>
       <c r="B18" s="28"/>
-      <c r="C18" s="59" t="str">
+      <c r="C18" s="51" t="str">
         <f>IF(F16="LEGAL","R.U.C","Consorciados separados por comas")</f>
         <v>Consorciados separados por comas</v>
       </c>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="60" t="str">
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="52" t="str">
         <f>IF(F16="LEGAL","","EMPRESA 1, EMPRESA 2")</f>
         <v>EMPRESA 1, EMPRESA 2</v>
       </c>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
       <c r="I18" s="28"/>
       <c r="J18" s="34"/>
       <c r="K18" s="28"/>
       <c r="L18" s="44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M18" s="44"/>
       <c r="N18" s="44"/>
-      <c r="O18" s="46" t="s">
+      <c r="O18" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="P18" s="46"/>
-      <c r="Q18" s="46"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="50"/>
       <c r="R18" s="28"/>
       <c r="S18" s="34"/>
       <c r="T18" s="28"/>
       <c r="U18" s="44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V18" s="44"/>
       <c r="W18" s="44"/>
-      <c r="X18" s="63"/>
-      <c r="Y18" s="63"/>
-      <c r="Z18" s="63"/>
+      <c r="X18" s="48"/>
+      <c r="Y18" s="48"/>
+      <c r="Z18" s="48"/>
       <c r="AA18" s="28"/>
       <c r="AB18" s="34"/>
     </row>
     <row r="19" spans="1:28" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="34"/>
       <c r="B19" s="28"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
       <c r="I19" s="28"/>
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
@@ -3412,15 +3421,15 @@
       <c r="S19" s="34"/>
       <c r="T19" s="28"/>
       <c r="U19" s="44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="V19" s="44"/>
       <c r="W19" s="44"/>
-      <c r="X19" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y19" s="63"/>
-      <c r="Z19" s="63"/>
+      <c r="X19" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y19" s="48"/>
+      <c r="Z19" s="48"/>
       <c r="AA19" s="28"/>
       <c r="AB19" s="34"/>
     </row>
@@ -3428,13 +3437,13 @@
       <c r="A20" s="34"/>
       <c r="B20" s="28"/>
       <c r="C20" s="44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D20" s="44"/>
       <c r="E20" s="28"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
       <c r="I20" s="28"/>
       <c r="J20" s="34"/>
       <c r="K20" s="34"/>
@@ -3447,14 +3456,14 @@
       <c r="R20" s="34"/>
       <c r="S20" s="34"/>
       <c r="T20" s="28"/>
-      <c r="U20" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="V20" s="64"/>
-      <c r="W20" s="64"/>
-      <c r="X20" s="63"/>
-      <c r="Y20" s="63"/>
-      <c r="Z20" s="63"/>
+      <c r="U20" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="V20" s="49"/>
+      <c r="W20" s="49"/>
+      <c r="X20" s="48"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="48"/>
       <c r="AA20" s="28"/>
       <c r="AB20" s="34"/>
     </row>
@@ -3469,15 +3478,15 @@
       <c r="H21" s="34"/>
       <c r="I21" s="34"/>
       <c r="J21" s="34"/>
-      <c r="K21" s="55" t="s">
+      <c r="K21" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="L21" s="55"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="55"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="46"/>
+      <c r="Q21" s="46"/>
       <c r="R21" s="32"/>
       <c r="S21" s="37"/>
       <c r="T21" s="37"/>
@@ -3492,28 +3501,28 @@
     </row>
     <row r="22" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="34"/>
-      <c r="B22" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="55"/>
+      <c r="B22" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
       <c r="J22" s="34"/>
       <c r="K22" s="28"/>
       <c r="L22" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M22" s="44"/>
-      <c r="N22" s="58">
+      <c r="N22" s="61">
         <v>9564123.3599999994</v>
       </c>
-      <c r="O22" s="58"/>
-      <c r="P22" s="58"/>
-      <c r="Q22" s="58"/>
+      <c r="O22" s="61"/>
+      <c r="P22" s="61"/>
+      <c r="Q22" s="61"/>
       <c r="R22" s="28"/>
       <c r="S22" s="34"/>
       <c r="T22" s="34"/>
@@ -3530,7 +3539,7 @@
       <c r="A23" s="34"/>
       <c r="B23" s="28"/>
       <c r="C23" s="44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D23" s="44"/>
       <c r="E23" s="44"/>
@@ -3541,15 +3550,15 @@
       <c r="J23" s="34"/>
       <c r="K23" s="28"/>
       <c r="L23" s="44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M23" s="44"/>
-      <c r="N23" s="52">
+      <c r="N23" s="58">
         <v>9567120.3000000007</v>
       </c>
-      <c r="O23" s="52"/>
-      <c r="P23" s="52"/>
-      <c r="Q23" s="52"/>
+      <c r="O23" s="58"/>
+      <c r="P23" s="58"/>
+      <c r="Q23" s="58"/>
       <c r="R23" s="28"/>
       <c r="S23" s="34"/>
       <c r="T23" s="34"/>
@@ -3566,28 +3575,28 @@
       <c r="A24" s="34"/>
       <c r="B24" s="28"/>
       <c r="C24" s="44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D24" s="44"/>
       <c r="E24" s="44"/>
       <c r="F24" s="44"/>
-      <c r="G24" s="62">
+      <c r="G24" s="45">
         <v>20600692063</v>
       </c>
-      <c r="H24" s="62"/>
+      <c r="H24" s="45"/>
       <c r="I24" s="28"/>
       <c r="J24" s="34"/>
       <c r="K24" s="28"/>
       <c r="L24" s="44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M24" s="44"/>
-      <c r="N24" s="46">
+      <c r="N24" s="50">
         <v>1</v>
       </c>
-      <c r="O24" s="46"/>
-      <c r="P24" s="46"/>
-      <c r="Q24" s="46"/>
+      <c r="O24" s="50"/>
+      <c r="P24" s="50"/>
+      <c r="Q24" s="50"/>
       <c r="R24" s="28"/>
       <c r="S24" s="34"/>
       <c r="T24" s="34"/>
@@ -3604,28 +3613,28 @@
       <c r="A25" s="34"/>
       <c r="B25" s="28"/>
       <c r="C25" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D25" s="42"/>
       <c r="E25" s="42"/>
       <c r="F25" s="42"/>
-      <c r="G25" s="45" t="s">
+      <c r="G25" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="H25" s="45"/>
+      <c r="H25" s="43"/>
       <c r="I25" s="28"/>
       <c r="J25" s="34"/>
       <c r="K25" s="28"/>
       <c r="L25" s="44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M25" s="44"/>
-      <c r="N25" s="61">
+      <c r="N25" s="54">
         <v>10789456.65</v>
       </c>
-      <c r="O25" s="61"/>
-      <c r="P25" s="61"/>
-      <c r="Q25" s="61"/>
+      <c r="O25" s="54"/>
+      <c r="P25" s="54"/>
+      <c r="Q25" s="54"/>
       <c r="R25" s="28"/>
       <c r="S25" s="34"/>
       <c r="T25" s="34"/>
@@ -3642,7 +3651,7 @@
       <c r="A26" s="34"/>
       <c r="B26" s="28"/>
       <c r="C26" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D26" s="44"/>
       <c r="E26" s="44"/>
@@ -3653,15 +3662,15 @@
       <c r="J26" s="34"/>
       <c r="K26" s="28"/>
       <c r="L26" s="44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M26" s="44"/>
-      <c r="N26" s="46" t="s">
+      <c r="N26" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="O26" s="46"/>
-      <c r="P26" s="46"/>
-      <c r="Q26" s="46"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="50"/>
       <c r="R26" s="28"/>
       <c r="S26" s="34"/>
       <c r="T26" s="34"/>
@@ -3678,28 +3687,28 @@
       <c r="A27" s="34"/>
       <c r="B27" s="28"/>
       <c r="C27" s="44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D27" s="44"/>
       <c r="E27" s="44"/>
       <c r="F27" s="44"/>
-      <c r="G27" s="62">
+      <c r="G27" s="45">
         <v>20600692063</v>
       </c>
-      <c r="H27" s="62"/>
+      <c r="H27" s="45"/>
       <c r="I27" s="28"/>
       <c r="J27" s="34"/>
       <c r="K27" s="28"/>
       <c r="L27" s="44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M27" s="44"/>
-      <c r="N27" s="50">
+      <c r="N27" s="53">
         <v>0.2</v>
       </c>
-      <c r="O27" s="50"/>
-      <c r="P27" s="50"/>
-      <c r="Q27" s="50"/>
+      <c r="O27" s="53"/>
+      <c r="P27" s="53"/>
+      <c r="Q27" s="53"/>
       <c r="R27" s="28"/>
       <c r="S27" s="34"/>
       <c r="T27" s="34"/>
@@ -3716,28 +3725,28 @@
       <c r="A28" s="34"/>
       <c r="B28" s="28"/>
       <c r="C28" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D28" s="42"/>
       <c r="E28" s="42"/>
       <c r="F28" s="42"/>
-      <c r="G28" s="45" t="s">
+      <c r="G28" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="H28" s="45"/>
+      <c r="H28" s="43"/>
       <c r="I28" s="28"/>
       <c r="J28" s="34"/>
       <c r="K28" s="28"/>
       <c r="L28" s="44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M28" s="44"/>
-      <c r="N28" s="50">
+      <c r="N28" s="53">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="O28" s="50"/>
-      <c r="P28" s="50"/>
-      <c r="Q28" s="50"/>
+      <c r="O28" s="53"/>
+      <c r="P28" s="53"/>
+      <c r="Q28" s="53"/>
       <c r="R28" s="28"/>
       <c r="S28" s="34"/>
       <c r="T28" s="34"/>
@@ -3754,7 +3763,7 @@
       <c r="A29" s="34"/>
       <c r="B29" s="28"/>
       <c r="C29" s="44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D29" s="44"/>
       <c r="E29" s="44"/>
@@ -3765,15 +3774,15 @@
       <c r="J29" s="34"/>
       <c r="K29" s="28"/>
       <c r="L29" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M29" s="44"/>
-      <c r="N29" s="50">
+      <c r="N29" s="53">
         <v>0.18</v>
       </c>
-      <c r="O29" s="50"/>
-      <c r="P29" s="50"/>
-      <c r="Q29" s="50"/>
+      <c r="O29" s="53"/>
+      <c r="P29" s="53"/>
+      <c r="Q29" s="53"/>
       <c r="R29" s="28"/>
       <c r="S29" s="34"/>
       <c r="T29" s="34"/>
@@ -3790,28 +3799,28 @@
       <c r="A30" s="34"/>
       <c r="B30" s="28"/>
       <c r="C30" s="44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D30" s="44"/>
       <c r="E30" s="44"/>
       <c r="F30" s="44"/>
-      <c r="G30" s="62">
+      <c r="G30" s="45">
         <v>20600692063</v>
       </c>
-      <c r="H30" s="62"/>
+      <c r="H30" s="45"/>
       <c r="I30" s="28"/>
       <c r="J30" s="34"/>
       <c r="K30" s="28"/>
       <c r="L30" s="44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M30" s="44"/>
-      <c r="N30" s="50">
+      <c r="N30" s="53">
         <v>0.18</v>
       </c>
-      <c r="O30" s="50"/>
-      <c r="P30" s="50"/>
-      <c r="Q30" s="50"/>
+      <c r="O30" s="53"/>
+      <c r="P30" s="53"/>
+      <c r="Q30" s="53"/>
       <c r="R30" s="28"/>
       <c r="S30" s="34"/>
       <c r="T30" s="34"/>
@@ -3828,15 +3837,15 @@
       <c r="A31" s="34"/>
       <c r="B31" s="28"/>
       <c r="C31" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D31" s="42"/>
       <c r="E31" s="42"/>
       <c r="F31" s="42"/>
-      <c r="G31" s="45" t="s">
+      <c r="G31" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="H31" s="45"/>
+      <c r="H31" s="43"/>
       <c r="I31" s="28"/>
       <c r="J31" s="34"/>
       <c r="K31" s="34"/>
@@ -3862,7 +3871,7 @@
       <c r="A32" s="34"/>
       <c r="B32" s="28"/>
       <c r="C32" s="44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D32" s="44"/>
       <c r="E32" s="44"/>
@@ -3872,15 +3881,15 @@
       <c r="I32" s="28"/>
       <c r="J32" s="34"/>
       <c r="K32" s="32"/>
-      <c r="L32" s="55" t="s">
-        <v>64</v>
-      </c>
-      <c r="M32" s="55"/>
-      <c r="N32" s="55"/>
-      <c r="O32" s="55"/>
-      <c r="P32" s="55"/>
-      <c r="Q32" s="55"/>
-      <c r="R32" s="55"/>
+      <c r="L32" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="M32" s="46"/>
+      <c r="N32" s="46"/>
+      <c r="O32" s="46"/>
+      <c r="P32" s="46"/>
+      <c r="Q32" s="46"/>
+      <c r="R32" s="46"/>
       <c r="S32" s="34"/>
       <c r="T32" s="34"/>
       <c r="U32" s="34"/>
@@ -3896,29 +3905,29 @@
       <c r="A33" s="34"/>
       <c r="B33" s="28"/>
       <c r="C33" s="44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D33" s="44"/>
       <c r="E33" s="44"/>
       <c r="F33" s="44"/>
-      <c r="G33" s="62">
+      <c r="G33" s="45">
         <v>20600692063</v>
       </c>
-      <c r="H33" s="62"/>
+      <c r="H33" s="45"/>
       <c r="I33" s="28"/>
       <c r="J33" s="34"/>
       <c r="K33" s="28"/>
-      <c r="L33" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="M33" s="51"/>
-      <c r="N33" s="52">
+      <c r="L33" s="57" t="s">
+        <v>88</v>
+      </c>
+      <c r="M33" s="57"/>
+      <c r="N33" s="58">
         <f>(10/100)*N23</f>
         <v>956712.03000000014</v>
       </c>
-      <c r="O33" s="52"/>
-      <c r="P33" s="52"/>
-      <c r="Q33" s="52"/>
+      <c r="O33" s="58"/>
+      <c r="P33" s="58"/>
+      <c r="Q33" s="58"/>
       <c r="R33" s="41"/>
       <c r="S33" s="34"/>
       <c r="T33" s="34"/>
@@ -3935,24 +3944,24 @@
       <c r="A34" s="34"/>
       <c r="B34" s="28"/>
       <c r="C34" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D34" s="42"/>
       <c r="E34" s="42"/>
       <c r="F34" s="42"/>
-      <c r="G34" s="45" t="s">
+      <c r="G34" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="H34" s="45"/>
+      <c r="H34" s="43"/>
       <c r="I34" s="28"/>
       <c r="J34" s="34"/>
       <c r="K34" s="28"/>
-      <c r="L34" s="51"/>
-      <c r="M34" s="51"/>
-      <c r="N34" s="52"/>
-      <c r="O34" s="52"/>
-      <c r="P34" s="52"/>
-      <c r="Q34" s="52"/>
+      <c r="L34" s="57"/>
+      <c r="M34" s="57"/>
+      <c r="N34" s="58"/>
+      <c r="O34" s="58"/>
+      <c r="P34" s="58"/>
+      <c r="Q34" s="58"/>
       <c r="R34" s="41"/>
       <c r="S34" s="34"/>
       <c r="T34" s="34"/>
@@ -3978,12 +3987,12 @@
       <c r="J35" s="34"/>
       <c r="K35" s="34"/>
       <c r="L35" s="34"/>
-      <c r="M35" s="53"/>
-      <c r="N35" s="53"/>
-      <c r="O35" s="54"/>
-      <c r="P35" s="54"/>
-      <c r="Q35" s="54"/>
-      <c r="R35" s="54"/>
+      <c r="M35" s="59"/>
+      <c r="N35" s="59"/>
+      <c r="O35" s="60"/>
+      <c r="P35" s="60"/>
+      <c r="Q35" s="60"/>
+      <c r="R35" s="60"/>
       <c r="S35" s="34"/>
       <c r="T35" s="34"/>
       <c r="U35" s="34"/>
@@ -3997,15 +4006,91 @@
     </row>
   </sheetData>
   <mergeCells count="118">
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="X17:Z17"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="U4:W4"/>
+    <mergeCell ref="X4:Z4"/>
+    <mergeCell ref="X5:Z7"/>
+    <mergeCell ref="U5:W7"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:Q30"/>
+    <mergeCell ref="N24:Q24"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="K21:Q21"/>
+    <mergeCell ref="T16:AA16"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="L33:M34"/>
+    <mergeCell ref="N33:Q34"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="O35:R35"/>
+    <mergeCell ref="T2:AA2"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="N22:Q22"/>
+    <mergeCell ref="N23:Q23"/>
+    <mergeCell ref="K2:Q2"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="O14:Q14"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="C18:E19"/>
+    <mergeCell ref="F18:H19"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="N29:Q29"/>
+    <mergeCell ref="N25:Q25"/>
+    <mergeCell ref="N26:Q26"/>
+    <mergeCell ref="N27:Q27"/>
+    <mergeCell ref="N28:Q28"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="B22:I22"/>
     <mergeCell ref="L32:R32"/>
     <mergeCell ref="T10:AA10"/>
     <mergeCell ref="C23:F23"/>
@@ -4030,91 +4115,15 @@
     <mergeCell ref="X19:Z19"/>
     <mergeCell ref="U20:W20"/>
     <mergeCell ref="X20:Z20"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="C18:E19"/>
-    <mergeCell ref="F18:H19"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="N29:Q29"/>
-    <mergeCell ref="N25:Q25"/>
-    <mergeCell ref="N26:Q26"/>
-    <mergeCell ref="N27:Q27"/>
-    <mergeCell ref="N28:Q28"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="K2:Q2"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="O13:Q13"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="O14:Q14"/>
-    <mergeCell ref="O15:Q15"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L33:M34"/>
-    <mergeCell ref="N33:Q34"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="O35:R35"/>
-    <mergeCell ref="T2:AA2"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="N22:Q22"/>
-    <mergeCell ref="N23:Q23"/>
-    <mergeCell ref="X17:Z17"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="U4:W4"/>
-    <mergeCell ref="X4:Z4"/>
-    <mergeCell ref="X5:Z7"/>
-    <mergeCell ref="U5:W7"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:Q30"/>
-    <mergeCell ref="N24:Q24"/>
-    <mergeCell ref="O16:Q16"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="O17:Q17"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="K21:Q21"/>
-    <mergeCell ref="T16:AA16"/>
-    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G33:H33"/>
   </mergeCells>
   <dataValidations count="14">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="El número de colegiatura admite solo numeros" sqref="G24:H24 G27:H27 G30:H30 G33:H33" xr:uid="{BA6FDD6D-E656-4FAF-9D05-EC68B04D8BC0}">
@@ -5362,7 +5371,7 @@
       <c r="E1" s="70"/>
       <c r="F1" s="70"/>
       <c r="G1" s="74" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" s="75"/>
       <c r="I1" s="75"/>
@@ -31638,46 +31647,51 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8489288-DE01-440D-9DCF-D61E4CA0CE56}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" hidden="1"/>
+    <col min="2" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="B1" s="77"/>
       <c r="C1" s="77"/>
       <c r="D1" s="77"/>
       <c r="E1" s="77"/>
       <c r="F1" s="77"/>
-    </row>
-    <row r="2" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="77"/>
+    </row>
+    <row r="2" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77"/>
       <c r="B2" s="77"/>
       <c r="C2" s="77"/>
       <c r="D2" s="77"/>
       <c r="E2" s="77"/>
       <c r="F2" s="77"/>
-    </row>
-    <row r="3" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="77"/>
+    </row>
+    <row r="3" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="78"/>
       <c r="B3" s="78"/>
       <c r="C3" s="78"/>
       <c r="D3" s="78"/>
       <c r="E3" s="78"/>
       <c r="F3" s="78"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="78"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="79" t="s">
         <v>39</v>
       </c>
@@ -31685,9 +31699,10 @@
       <c r="C4" s="80"/>
       <c r="D4" s="80"/>
       <c r="E4" s="80"/>
-      <c r="F4" s="81"/>
-    </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="80"/>
+      <c r="G4" s="81"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>33</v>
       </c>
@@ -31706,12 +31721,311 @@
       <c r="F5" s="30" t="s">
         <v>38</v>
       </c>
+      <c r="G5" s="82" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="83"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="83"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="83"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="83"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="83"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="83"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="83"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="83"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="83"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="83"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="83"/>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="83"/>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="83"/>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="83"/>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="83"/>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="83"/>
+    </row>
+    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="83"/>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="83"/>
+    </row>
+    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="83"/>
+    </row>
+    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="83"/>
+    </row>
+    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="83"/>
+    </row>
+    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="83"/>
+    </row>
+    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="83"/>
+    </row>
+    <row r="30" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="83"/>
+    </row>
+    <row r="31" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="83"/>
+    </row>
+    <row r="32" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="83"/>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="83"/>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="83"/>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="83"/>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="83"/>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="83"/>
+    </row>
+    <row r="38" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="83"/>
+    </row>
+    <row r="39" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G39" s="83"/>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G40" s="83"/>
+    </row>
+    <row r="41" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G41" s="83"/>
+    </row>
+    <row r="42" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G42" s="83"/>
+    </row>
+    <row r="43" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G43" s="83"/>
+    </row>
+    <row r="44" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G44" s="83"/>
+    </row>
+    <row r="45" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G45" s="83"/>
+    </row>
+    <row r="46" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G46" s="83"/>
+    </row>
+    <row r="47" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G47" s="83"/>
+    </row>
+    <row r="48" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G48" s="83"/>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G49" s="83"/>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G50" s="83"/>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G51" s="83"/>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G52" s="83"/>
+    </row>
+    <row r="53" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G53" s="83"/>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G54" s="83"/>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G55" s="83"/>
+    </row>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G56" s="83"/>
+    </row>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G57" s="83"/>
+    </row>
+    <row r="58" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G58" s="83"/>
+    </row>
+    <row r="59" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G59" s="83"/>
+    </row>
+    <row r="60" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G60" s="83"/>
+    </row>
+    <row r="61" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G61" s="83"/>
+    </row>
+    <row r="62" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G62" s="83"/>
+    </row>
+    <row r="63" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G63" s="83"/>
+    </row>
+    <row r="64" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G64" s="83"/>
+    </row>
+    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G65" s="83"/>
+    </row>
+    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G66" s="83"/>
+    </row>
+    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G67" s="83"/>
+    </row>
+    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G68" s="83"/>
+    </row>
+    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G69" s="83"/>
+    </row>
+    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G70" s="83"/>
+    </row>
+    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G71" s="83"/>
+    </row>
+    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G72" s="83"/>
+    </row>
+    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G73" s="83"/>
+    </row>
+    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G74" s="83"/>
+    </row>
+    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G75" s="83"/>
+    </row>
+    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G76" s="83"/>
+    </row>
+    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G77" s="83"/>
+    </row>
+    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G78" s="83"/>
+    </row>
+    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G79" s="83"/>
+    </row>
+    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G80" s="83"/>
+    </row>
+    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G81" s="83"/>
+    </row>
+    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G82" s="83"/>
+    </row>
+    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G83" s="83"/>
+    </row>
+    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G84" s="83"/>
+    </row>
+    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G85" s="83"/>
+    </row>
+    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G86" s="83"/>
+    </row>
+    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G87" s="83"/>
+    </row>
+    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G88" s="83"/>
+    </row>
+    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G89" s="83"/>
+    </row>
+    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G90" s="83"/>
+    </row>
+    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G91" s="83"/>
+    </row>
+    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G92" s="83"/>
+    </row>
+    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G93" s="83"/>
+    </row>
+    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G94" s="83"/>
+    </row>
+    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G95" s="83"/>
+    </row>
+    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G96" s="83"/>
+    </row>
+    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G97" s="83"/>
+    </row>
+    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G98" s="83"/>
+    </row>
+    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G99" s="83"/>
+    </row>
+    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G100" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:F3"/>
-    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A1:G3"/>
+    <mergeCell ref="A4:G4"/>
   </mergeCells>
+  <conditionalFormatting sqref="G6:G100">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>